<commit_message>
This is kind of a superfluous commit but I'd rather get everything done
</commit_message>
<xml_diff>
--- a/Suivis.xlsx
+++ b/Suivis.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\School_Related\Session_3\Prog_2D_Avancé\TP_FINAL_I_E\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\School\Everything\Inhospitable Enviro\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Date</t>
   </si>
@@ -36,12 +36,78 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Création de l'UML</t>
+  </si>
+  <si>
+    <t>Trouvé concept</t>
+  </si>
+  <si>
+    <t>Préparations des classes</t>
+  </si>
+  <si>
+    <t>setup des niveaux</t>
+  </si>
+  <si>
+    <t>debugging</t>
+  </si>
+  <si>
+    <t>creation du endscreen</t>
+  </si>
+  <si>
+    <t>implementation des animations</t>
+  </si>
+  <si>
+    <t>decoupage de sprites</t>
+  </si>
+  <si>
+    <t>creation des animations</t>
+  </si>
+  <si>
+    <t>debugging du personnage</t>
+  </si>
+  <si>
+    <t>amelioration du movement du personnage</t>
+  </si>
+  <si>
+    <t>implemation d'un delegate simple</t>
+  </si>
+  <si>
+    <t>implementation des son et musics</t>
+  </si>
+  <si>
+    <t>essai d'implentation de la localisation (MUST FINISH)</t>
+  </si>
+  <si>
+    <t>finission du start screen</t>
+  </si>
+  <si>
+    <t>implemenation de la mort et du system de vie du perso</t>
+  </si>
+  <si>
+    <t>implementation du movement du perso</t>
+  </si>
+  <si>
+    <t>setup du niveau initial</t>
+  </si>
+  <si>
+    <t>creation du start screen</t>
+  </si>
+  <si>
+    <t>implementation des échelles</t>
+  </si>
+  <si>
+    <t>overhaul de sons</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy/mm/dd"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -79,7 +145,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -96,17 +162,20 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
-      <numFmt numFmtId="19" formatCode="yyyy/mm/dd"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
+      <numFmt numFmtId="164" formatCode="yyyy/mm/dd"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
@@ -123,19 +192,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B2:D14" totalsRowShown="0">
-  <autoFilter ref="B2:D14"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B2:D28" totalsRowShown="0">
+  <autoFilter ref="B2:D28"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Date" dataDxfId="0"/>
+    <tableColumn id="1" name="Date" dataDxfId="1"/>
     <tableColumn id="2" name="Tâche"/>
-    <tableColumn id="3" name="Temps" dataDxfId="1"/>
+    <tableColumn id="3" name="Temps" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -397,13 +466,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D14"/>
+  <dimension ref="B2:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="16.85546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="54" customWidth="1"/>
@@ -422,57 +491,234 @@
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="2"/>
-      <c r="D3" s="4"/>
+      <c r="B3" s="2">
+        <v>42203</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="4">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="2"/>
-      <c r="D4" s="4"/>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="2"/>
-      <c r="D5" s="4"/>
+      <c r="B5" s="2">
+        <v>42207</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="4">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
-      <c r="D6" s="4"/>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="4">
+        <v>2</v>
+      </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="2"/>
-      <c r="D7" s="4"/>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" s="2"/>
-      <c r="D8" s="4"/>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" s="2"/>
-      <c r="D9" s="4"/>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="4">
+        <v>2</v>
+      </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" s="2"/>
       <c r="D10" s="4"/>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="2"/>
-      <c r="D11" s="4"/>
+      <c r="B11" s="2">
+        <v>42210</v>
+      </c>
+      <c r="C11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="4">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" s="2"/>
-      <c r="D12" s="4"/>
+      <c r="C12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="4">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" s="2"/>
-      <c r="D13" s="4"/>
-    </row>
-    <row r="14" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14" s="2"/>
-      <c r="C14" s="3" t="s">
+      <c r="D14" s="4"/>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B15" s="2"/>
+      <c r="D15" s="4"/>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B16" s="2">
+        <v>42211</v>
+      </c>
+      <c r="C16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="2"/>
+      <c r="C17" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="2">
+        <v>42212</v>
+      </c>
+      <c r="C18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="2"/>
+      <c r="C19" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" s="4">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="2"/>
+      <c r="C20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="2"/>
+      <c r="C21" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="2"/>
+      <c r="D22" s="4"/>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="2">
+        <v>42213</v>
+      </c>
+      <c r="C23" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B24" s="2"/>
+      <c r="C24" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B25" s="2"/>
+      <c r="C25" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="6">
+        <v>42215</v>
+      </c>
+      <c r="C26" t="s">
+        <v>24</v>
+      </c>
+      <c r="D26" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27" s="2">
+        <v>42216</v>
+      </c>
+      <c r="C27" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" s="4">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B28" s="2"/>
+      <c r="C28" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D14" s="5">
-        <f>SUBTOTAL(109,D3:D13)</f>
-        <v>0</v>
+      <c r="D28" s="5">
+        <f>SUBTOTAL(109,D3:D27)</f>
+        <v>40.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>